<commit_message>
added excel file for test cases
</commit_message>
<xml_diff>
--- a/Test cases.xlsx
+++ b/Test cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_sample_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_sample_project\NopCommercePytest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B597995-729F-421D-853F-53D1E67B9A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BDDF7B-C22C-4F73-BA3D-4C8803C68314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,25 +286,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,7 +641,7 @@
       <c r="A2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -663,14 +663,16 @@
     </row>
     <row r="3" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
-      <c r="B3" s="10"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -941,115 +943,120 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="15" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="11"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="11"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="12"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="11"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="C2:C7"/>
     <mergeCell ref="L2:L7"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="G2:G7"/>
@@ -1057,11 +1064,6 @@
     <mergeCell ref="J2:J7"/>
     <mergeCell ref="I2:I7"/>
     <mergeCell ref="H2:H7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="C2:C7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="RTM!A2" display="TC-101" xr:uid="{D284F41A-3515-49DD-9E4E-DCB5E1FCD4EA}"/>

</xml_diff>